<commit_message>
- moved skip if complete and failed logic one indent inside the for  loop - deleted autoast_indexing after copying it and naming it V2 Cuisinart_Dev.py
</commit_message>
<xml_diff>
--- a/autoast/alan_jobs.xlsx
+++ b/autoast/alan_jobs.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -29,12 +29,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <color rgb="FF000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
       <sz val="11"/>
     </font>
     <font>
@@ -101,7 +95,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -109,36 +103,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
@@ -151,11 +142,8 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -558,235 +546,237 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="23.57642857142857" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
-    <col width="138.8621428571429" bestFit="1" customWidth="1" style="7" min="2" max="2"/>
-    <col width="17.71928571428571" bestFit="1" customWidth="1" style="18" min="3" max="3"/>
-    <col width="16.86214285714286" bestFit="1" customWidth="1" style="7" min="4" max="4"/>
-    <col width="17.29071428571428" bestFit="1" customWidth="1" style="7" min="5" max="5"/>
-    <col width="110.4335714285714" bestFit="1" customWidth="1" style="6" min="6" max="6"/>
-    <col width="29.29071428571428" bestFit="1" customWidth="1" style="7" min="7" max="7"/>
-    <col width="20.57642857142857" bestFit="1" customWidth="1" style="19" min="8" max="8"/>
-    <col width="25.57642857142857" bestFit="1" customWidth="1" style="18" min="9" max="9"/>
-    <col width="21.005" bestFit="1" customWidth="1" style="18" min="10" max="10"/>
-    <col width="21.29071428571428" bestFit="1" customWidth="1" style="7" min="11" max="11"/>
-    <col width="13.71928571428571" bestFit="1" customWidth="1" style="18" min="12" max="12"/>
-    <col width="14.71928571428571" bestFit="1" customWidth="1" style="7" min="13" max="13"/>
-    <col width="11.57642857142857" bestFit="1" customWidth="1" style="7" min="14" max="14"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="15" max="15"/>
+    <col width="23.57642857142857" bestFit="1" customWidth="1" style="6" min="1" max="1"/>
+    <col width="138.8621428571429" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
+    <col width="17.71928571428571" bestFit="1" customWidth="1" style="16" min="3" max="3"/>
+    <col width="16.86214285714286" bestFit="1" customWidth="1" style="6" min="4" max="4"/>
+    <col width="17.29071428571428" bestFit="1" customWidth="1" style="6" min="5" max="5"/>
+    <col width="110.4335714285714" bestFit="1" customWidth="1" style="5" min="6" max="6"/>
+    <col width="29.29071428571428" bestFit="1" customWidth="1" style="6" min="7" max="7"/>
+    <col width="20.57642857142857" bestFit="1" customWidth="1" style="17" min="8" max="8"/>
+    <col width="25.57642857142857" bestFit="1" customWidth="1" style="16" min="9" max="9"/>
+    <col width="21.005" bestFit="1" customWidth="1" style="16" min="10" max="10"/>
+    <col width="21.29071428571428" bestFit="1" customWidth="1" style="6" min="11" max="11"/>
+    <col width="13.71928571428571" bestFit="1" customWidth="1" style="16" min="12" max="12"/>
+    <col width="14.71928571428571" bestFit="1" customWidth="1" style="6" min="13" max="13"/>
+    <col width="11.57642857142857" bestFit="1" customWidth="1" style="6" min="14" max="14"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>region</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>feature_layer</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>crown_file_number</t>
         </is>
       </c>
-      <c r="D1" s="9" t="inlineStr">
+      <c r="D1" s="8" t="inlineStr">
         <is>
           <t>disposition_number</t>
         </is>
       </c>
-      <c r="E1" s="9" t="inlineStr">
+      <c r="E1" s="8" t="inlineStr">
         <is>
           <t>parcel_number</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>output_directory</t>
         </is>
       </c>
-      <c r="G1" s="10" t="inlineStr">
+      <c r="G1" s="9" t="inlineStr">
         <is>
           <t>output_directory_same_as_input</t>
         </is>
       </c>
-      <c r="H1" s="10" t="inlineStr">
+      <c r="H1" s="9" t="inlineStr">
         <is>
           <t>dont_overwrite_outputs</t>
         </is>
       </c>
-      <c r="I1" s="11" t="inlineStr">
+      <c r="I1" s="10" t="inlineStr">
         <is>
           <t>skip_conflicts_and_constraints</t>
         </is>
       </c>
-      <c r="J1" s="11" t="inlineStr">
+      <c r="J1" s="10" t="inlineStr">
         <is>
           <t>suppress_map_creation</t>
         </is>
       </c>
-      <c r="K1" s="10" t="inlineStr">
+      <c r="K1" s="9" t="inlineStr">
         <is>
           <t>add_maps_to_current</t>
         </is>
       </c>
-      <c r="L1" s="11" t="inlineStr">
+      <c r="L1" s="10" t="inlineStr">
         <is>
           <t>run_as_fcbc</t>
         </is>
       </c>
-      <c r="M1" s="4" t="inlineStr">
+      <c r="M1" s="3" t="inlineStr">
         <is>
           <t>ast_condition</t>
         </is>
       </c>
-      <c r="N1" s="9" t="inlineStr">
+      <c r="N1" s="8" t="inlineStr">
         <is>
           <t>file_number</t>
         </is>
       </c>
-      <c r="O1" s="9" t="n"/>
+      <c r="O1" s="8" t="n"/>
     </row>
     <row r="2" ht="19.5" customHeight="1">
-      <c r="A2" s="4" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>Northeast</t>
         </is>
       </c>
-      <c r="B2" s="12" t="inlineStr">
+      <c r="B2" s="11" t="inlineStr">
         <is>
           <t>W:\srm\wml\Workarea\Authorizations\Land\Northeast\8014576\Site_1.shp</t>
         </is>
       </c>
-      <c r="C2" s="8" t="inlineStr">
+      <c r="C2" s="7" t="inlineStr">
         <is>
           <t>8014576</t>
         </is>
       </c>
-      <c r="D2" s="13" t="n"/>
-      <c r="E2" s="13" t="n"/>
-      <c r="F2" s="12" t="inlineStr">
+      <c r="D2" s="12" t="n"/>
+      <c r="E2" s="12" t="n"/>
+      <c r="F2" s="11" t="inlineStr">
         <is>
           <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS\Site1</t>
         </is>
       </c>
-      <c r="G2" s="10" t="inlineStr">
+      <c r="G2" s="9" t="inlineStr">
         <is>
           <t>false</t>
         </is>
       </c>
-      <c r="H2" s="10" t="inlineStr">
+      <c r="H2" s="9" t="inlineStr">
         <is>
           <t>false</t>
         </is>
       </c>
-      <c r="I2" s="11" t="b">
+      <c r="I2" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="J2" s="11" t="b">
+      <c r="J2" s="10" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K2" s="9" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="L2" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="K2" s="10" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L2" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" s="14" t="inlineStr">
-        <is>
-          <t>COMPLETE</t>
-        </is>
-      </c>
-      <c r="N2" s="15" t="n"/>
-      <c r="O2" s="9" t="n"/>
+      <c r="M2" s="13" t="inlineStr">
+        <is>
+          <t>Queued</t>
+        </is>
+      </c>
+      <c r="N2" s="14" t="n"/>
+      <c r="O2" s="8" t="n"/>
     </row>
     <row r="3" ht="19.5" customHeight="1">
-      <c r="A3" s="4" t="n"/>
-      <c r="B3" s="12" t="n"/>
-      <c r="C3" s="13" t="n"/>
-      <c r="D3" s="13" t="n"/>
-      <c r="E3" s="13" t="n"/>
-      <c r="F3" s="12" t="n"/>
-      <c r="G3" s="10" t="n"/>
-      <c r="H3" s="10" t="n"/>
-      <c r="I3" s="16" t="n"/>
-      <c r="J3" s="16" t="n"/>
-      <c r="K3" s="10" t="n"/>
-      <c r="L3" s="16" t="n"/>
-      <c r="M3" s="4" t="n"/>
-      <c r="N3" s="15" t="n"/>
-      <c r="O3" s="9" t="n"/>
+      <c r="A3" s="3" t="n"/>
+      <c r="B3" s="11" t="n"/>
+      <c r="C3" s="12" t="n"/>
+      <c r="D3" s="12" t="n"/>
+      <c r="E3" s="12" t="n"/>
+      <c r="F3" s="11" t="n"/>
+      <c r="G3" s="9" t="n"/>
+      <c r="H3" s="9" t="n"/>
+      <c r="I3" s="15" t="n"/>
+      <c r="J3" s="15" t="n"/>
+      <c r="K3" s="9" t="n"/>
+      <c r="L3" s="15" t="n"/>
+      <c r="M3" s="3" t="n"/>
+      <c r="N3" s="14" t="n"/>
+      <c r="O3" s="8" t="n"/>
     </row>
     <row r="4" ht="19.5" customHeight="1">
-      <c r="A4" s="4" t="n"/>
-      <c r="B4" s="4" t="n"/>
-      <c r="C4" s="13" t="n"/>
-      <c r="D4" s="13" t="n"/>
-      <c r="E4" s="13" t="n"/>
-      <c r="F4" s="12" t="n"/>
-      <c r="G4" s="10" t="n"/>
-      <c r="H4" s="10" t="n"/>
-      <c r="I4" s="16" t="n"/>
-      <c r="J4" s="16" t="n"/>
-      <c r="K4" s="10" t="n"/>
-      <c r="L4" s="16" t="n"/>
-      <c r="M4" s="4" t="n"/>
-      <c r="N4" s="15" t="n"/>
-      <c r="O4" s="4" t="n"/>
+      <c r="A4" s="3" t="n"/>
+      <c r="B4" s="3" t="n"/>
+      <c r="C4" s="12" t="n"/>
+      <c r="D4" s="12" t="n"/>
+      <c r="E4" s="12" t="n"/>
+      <c r="F4" s="11" t="n"/>
+      <c r="G4" s="9" t="n"/>
+      <c r="H4" s="9" t="n"/>
+      <c r="I4" s="15" t="n"/>
+      <c r="J4" s="15" t="n"/>
+      <c r="K4" s="9" t="n"/>
+      <c r="L4" s="15" t="n"/>
+      <c r="M4" s="3" t="n"/>
+      <c r="N4" s="14" t="n"/>
+      <c r="O4" s="3" t="n"/>
     </row>
     <row r="5" ht="19.5" customHeight="1">
-      <c r="A5" s="4" t="n"/>
-      <c r="B5" s="12" t="n"/>
-      <c r="C5" s="13" t="n"/>
-      <c r="D5" s="13" t="n"/>
-      <c r="E5" s="13" t="n"/>
-      <c r="F5" s="12" t="n"/>
-      <c r="G5" s="10" t="n"/>
-      <c r="H5" s="10" t="n"/>
-      <c r="I5" s="16" t="n"/>
-      <c r="J5" s="16" t="n"/>
-      <c r="K5" s="10" t="n"/>
-      <c r="L5" s="16" t="n"/>
-      <c r="M5" s="4" t="n"/>
-      <c r="N5" s="13" t="n"/>
-      <c r="O5" s="9" t="n"/>
+      <c r="A5" s="3" t="n"/>
+      <c r="B5" s="11" t="n"/>
+      <c r="C5" s="12" t="n"/>
+      <c r="D5" s="12" t="n"/>
+      <c r="E5" s="12" t="n"/>
+      <c r="F5" s="11" t="n"/>
+      <c r="G5" s="9" t="n"/>
+      <c r="H5" s="9" t="n"/>
+      <c r="I5" s="15" t="n"/>
+      <c r="J5" s="15" t="n"/>
+      <c r="K5" s="9" t="n"/>
+      <c r="L5" s="15" t="n"/>
+      <c r="M5" s="3" t="n"/>
+      <c r="N5" s="12" t="n"/>
+      <c r="O5" s="8" t="n"/>
     </row>
     <row r="6" ht="19.5" customHeight="1">
-      <c r="A6" s="7" t="n"/>
-      <c r="B6" s="7" t="n"/>
-      <c r="C6" s="17" t="n"/>
-      <c r="D6" s="7" t="n"/>
-      <c r="E6" s="7" t="n"/>
-      <c r="F6" s="12" t="n"/>
-      <c r="G6" s="10" t="n"/>
-      <c r="H6" s="10" t="n"/>
-      <c r="I6" s="16" t="n"/>
-      <c r="J6" s="16" t="n"/>
-      <c r="K6" s="10" t="n"/>
-      <c r="L6" s="16" t="n"/>
-      <c r="M6" s="13" t="n"/>
-      <c r="N6" s="13" t="n"/>
-      <c r="O6" s="13" t="n"/>
+      <c r="A6" s="6" t="n"/>
+      <c r="B6" s="6" t="n"/>
+      <c r="C6" s="12" t="n"/>
+      <c r="D6" s="6" t="n"/>
+      <c r="E6" s="6" t="n"/>
+      <c r="F6" s="11" t="n"/>
+      <c r="G6" s="9" t="n"/>
+      <c r="H6" s="9" t="n"/>
+      <c r="I6" s="15" t="n"/>
+      <c r="J6" s="15" t="n"/>
+      <c r="K6" s="9" t="n"/>
+      <c r="L6" s="15" t="n"/>
+      <c r="M6" s="12" t="n"/>
+      <c r="N6" s="12" t="n"/>
+      <c r="O6" s="12" t="n"/>
     </row>
     <row r="7" ht="19.5" customHeight="1">
-      <c r="A7" s="7" t="n"/>
-      <c r="B7" s="7" t="n"/>
-      <c r="C7" s="17" t="n"/>
-      <c r="D7" s="7" t="n"/>
-      <c r="E7" s="7" t="n"/>
-      <c r="F7" s="12" t="n"/>
-      <c r="G7" s="7" t="n"/>
-      <c r="H7" s="10" t="n"/>
-      <c r="I7" s="17" t="n"/>
-      <c r="J7" s="17" t="n"/>
-      <c r="K7" s="7" t="n"/>
-      <c r="L7" s="17" t="n"/>
-      <c r="M7" s="7" t="n"/>
-      <c r="N7" s="7" t="n"/>
-      <c r="O7" s="7" t="n"/>
+      <c r="A7" s="6" t="n"/>
+      <c r="B7" s="6" t="n"/>
+      <c r="C7" s="12" t="n"/>
+      <c r="D7" s="6" t="n"/>
+      <c r="E7" s="6" t="n"/>
+      <c r="F7" s="11" t="n"/>
+      <c r="G7" s="6" t="n"/>
+      <c r="H7" s="9" t="n"/>
+      <c r="I7" s="12" t="n"/>
+      <c r="J7" s="12" t="n"/>
+      <c r="K7" s="6" t="n"/>
+      <c r="L7" s="12" t="n"/>
+      <c r="M7" s="6" t="n"/>
+      <c r="N7" s="6" t="n"/>
+      <c r="O7" s="6" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -810,9 +800,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="27.14785714285714" bestFit="1" customWidth="1" style="6" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
+    <col width="27.14785714285714" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
@@ -821,8 +811,8 @@
           <t>Northeast</t>
         </is>
       </c>
-      <c r="B1" s="7" t="n"/>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="B1" s="6" t="n"/>
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>true</t>
         </is>
@@ -834,8 +824,8 @@
           <t>Cariboo</t>
         </is>
       </c>
-      <c r="B2" s="7" t="n"/>
-      <c r="C2" s="7" t="inlineStr">
+      <c r="B2" s="6" t="n"/>
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>false</t>
         </is>
@@ -847,17 +837,17 @@
           <t>Kootenay_Boundary</t>
         </is>
       </c>
-      <c r="B3" s="7" t="n"/>
-      <c r="C3" s="7" t="n"/>
+      <c r="B3" s="6" t="n"/>
+      <c r="C3" s="6" t="n"/>
     </row>
     <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="4" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>Skeena</t>
         </is>
       </c>
-      <c r="B4" s="7" t="n"/>
-      <c r="C4" s="7" t="n"/>
+      <c r="B4" s="6" t="n"/>
+      <c r="C4" s="6" t="n"/>
     </row>
     <row r="5" ht="18.75" customHeight="1">
       <c r="A5" s="1" t="inlineStr">
@@ -865,17 +855,17 @@
           <t>South_Coast</t>
         </is>
       </c>
-      <c r="B5" s="7" t="n"/>
-      <c r="C5" s="7" t="n"/>
+      <c r="B5" s="6" t="n"/>
+      <c r="C5" s="6" t="n"/>
     </row>
     <row r="6" ht="18.75" customHeight="1">
-      <c r="A6" s="4" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>Thompson_Okanagan</t>
         </is>
       </c>
-      <c r="B6" s="7" t="n"/>
-      <c r="C6" s="7" t="n"/>
+      <c r="B6" s="6" t="n"/>
+      <c r="C6" s="6" t="n"/>
     </row>
     <row r="7" ht="18.75" customHeight="1">
       <c r="A7" s="1" t="inlineStr">
@@ -883,17 +873,17 @@
           <t>West_Coast</t>
         </is>
       </c>
-      <c r="B7" s="7" t="n"/>
-      <c r="C7" s="7" t="n"/>
+      <c r="B7" s="6" t="n"/>
+      <c r="C7" s="6" t="n"/>
     </row>
     <row r="8" ht="18.75" customHeight="1">
-      <c r="A8" s="5" t="inlineStr">
+      <c r="A8" s="4" t="inlineStr">
         <is>
           <t>Omineca</t>
         </is>
       </c>
-      <c r="B8" s="7" t="n"/>
-      <c r="C8" s="7" t="n"/>
+      <c r="B8" s="6" t="n"/>
+      <c r="C8" s="6" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
reverted to the old set dont overwrite outputs to true, not contained in reload failed jobs. Added Save WB after it is set
</commit_message>
<xml_diff>
--- a/autoast/alan_jobs.xlsx
+++ b/autoast/alan_jobs.xlsx
@@ -95,7 +95,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -147,6 +147,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,7 +558,7 @@
     <col width="29.29071428571428" bestFit="1" customWidth="1" style="6" min="7" max="7"/>
     <col width="20.57642857142857" bestFit="1" customWidth="1" style="17" min="8" max="8"/>
     <col width="25.57642857142857" bestFit="1" customWidth="1" style="16" min="9" max="9"/>
-    <col width="21.005" bestFit="1" customWidth="1" style="16" min="10" max="10"/>
+    <col width="21.005" bestFit="1" customWidth="1" style="18" min="10" max="10"/>
     <col width="21.29071428571428" bestFit="1" customWidth="1" style="6" min="11" max="11"/>
     <col width="13.71928571428571" bestFit="1" customWidth="1" style="16" min="12" max="12"/>
     <col width="14.71928571428571" bestFit="1" customWidth="1" style="6" min="13" max="13"/>
@@ -609,7 +612,7 @@
           <t>skip_conflicts_and_constraints</t>
         </is>
       </c>
-      <c r="J1" s="10" t="inlineStr">
+      <c r="J1" s="9" t="inlineStr">
         <is>
           <t>suppress_map_creation</t>
         </is>
@@ -674,7 +677,7 @@
       </c>
       <c r="J2" s="10" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
       <c r="K2" s="9" t="inlineStr">

</xml_diff>